<commit_message>
Especificacao do caso de uso Tela Inicial
</commit_message>
<xml_diff>
--- a/Requisitos/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos/Requisitos e Casos de Uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>REQ#</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Descartar Alerta</t>
+  </si>
+  <si>
+    <t>Exibir os últimos/próximos eventos na tela inicial</t>
+  </si>
+  <si>
+    <t>Exibir Tela Inicial</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +683,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>29</v>
       </c>
@@ -686,6 +692,20 @@
       </c>
       <c r="D17" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diagrama de Classes Conceituais
</commit_message>
<xml_diff>
--- a/Requisitos/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos/Requisitos e Casos de Uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>REQ#</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Exibir Tela Inicial</t>
+  </si>
+  <si>
+    <t>Ao entrar no aplicativo, se existir mais de um bebê, perguntar ao usuário qual bebê deseja visualizar</t>
+  </si>
+  <si>
+    <t>Selecionar Bebê</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,6 +714,20 @@
         <v>33</v>
       </c>
     </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>